<commit_message>
corrected behavior for similar cluster names between cell types
</commit_message>
<xml_diff>
--- a/public/data/test_data_v2.xlsx
+++ b/public/data/test_data_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\miguel\dev\org-zhejiang\arabidopsis-reactjs\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5AED6-9A65-4D05-8D79-5E6A29A314EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED78F4-9C8B-4C8B-BC6D-A11A21425096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{557B7C7D-D8AB-43FF-9EEA-BBB0B6EEA029}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="77">
   <si>
     <t>Organelle</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Leaf pavement cell | log2FC_cluster 12</t>
+  </si>
+  <si>
+    <t>Mesophyll | log2FC_cluster 4</t>
   </si>
 </sst>
 </file>
@@ -5718,10 +5721,13 @@
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5746,7 +5752,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>71</v>

</xml_diff>